<commit_message>
work on Video - understanding discrepancy
Former-commit-id: 2d990192f4b76018894e3ba215b632785951ebfc
</commit_message>
<xml_diff>
--- a/Video/countries hdi.xlsx
+++ b/Video/countries hdi.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="4"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -48918,10 +48918,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48933,2015 +48933,2027 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1393</v>
+        <v>957</v>
       </c>
       <c r="B1" t="s">
-        <v>1228</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>0.77400000000000002</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>790</v>
+        <v>803</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>1120</v>
       </c>
       <c r="C2">
-        <v>0.84599999999999997</v>
+        <v>0.93300000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>791</v>
+        <v>956</v>
       </c>
       <c r="B3" t="s">
-        <v>1166</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>0.82699999999999996</v>
+        <v>0.92100000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>792</v>
+        <v>846</v>
       </c>
       <c r="B4" t="s">
-        <v>1119</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>0.46800000000000003</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>795</v>
+        <v>892</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>0.749</v>
+        <v>0.91600000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>796</v>
+        <v>987</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>0.72899999999999998</v>
+        <v>0.91600000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>798</v>
+        <v>1025</v>
       </c>
       <c r="B7" t="s">
-        <v>1190</v>
+        <v>1223</v>
       </c>
       <c r="C7">
-        <v>0.52600000000000002</v>
+        <v>0.91400000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>800</v>
+        <v>832</v>
       </c>
       <c r="B8" t="s">
-        <v>1244</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>0.80800000000000005</v>
+        <v>0.91300000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>802</v>
+        <v>961</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>1147</v>
       </c>
       <c r="C9">
-        <v>0.89500000000000002</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>803</v>
+        <v>899</v>
       </c>
       <c r="B10" t="s">
-        <v>1120</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>0.93300000000000005</v>
+        <v>0.90600000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>806</v>
+        <v>827</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>1224</v>
       </c>
       <c r="C11">
-        <v>0.73399999999999999</v>
+        <v>0.90200000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>807</v>
+        <v>848</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>0.73499999999999999</v>
+        <v>0.90100000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>808</v>
+        <v>988</v>
       </c>
       <c r="B13" t="s">
-        <v>1227</v>
+        <v>1157</v>
       </c>
       <c r="C13">
-        <v>0.77600000000000002</v>
+        <v>0.90100000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B14" t="s">
-        <v>1122</v>
+        <v>15</v>
       </c>
       <c r="C14">
-        <v>0.55800000000000005</v>
+        <v>0.89700000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <v>0.89700000000000002</v>
+        <v>0.89500000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>811</v>
+        <v>865</v>
       </c>
       <c r="B16" t="s">
-        <v>1216</v>
+        <v>19</v>
       </c>
       <c r="C16">
-        <v>0.38800000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.89300000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>812</v>
+        <v>860</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="C17">
-        <v>0.78200000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.89200000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>813</v>
+        <v>990</v>
       </c>
       <c r="B18" t="s">
-        <v>1121</v>
+        <v>23</v>
       </c>
       <c r="C18">
-        <v>0.81499999999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.89200000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>814</v>
+        <v>885</v>
       </c>
       <c r="B19" t="s">
-        <v>1215</v>
+        <v>1129</v>
       </c>
       <c r="C19">
-        <v>0.38900000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>815</v>
+        <v>912</v>
       </c>
       <c r="B20" t="s">
-        <v>1202</v>
+        <v>1159</v>
       </c>
       <c r="C20">
-        <v>0.47599999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>904</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C21">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>893</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C22">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>857</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>920</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>0.88300000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>900</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>867</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C26">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>925</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>845</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C28">
+        <v>0.873</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>879</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29">
+        <v>0.86</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>817</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B30" t="s">
         <v>1124</v>
       </c>
-      <c r="C21">
+      <c r="C30">
         <v>0.85199999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>818</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1250</v>
-      </c>
-      <c r="C22">
-        <v>0.66700000000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>820</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1247</v>
-      </c>
-      <c r="C23">
-        <v>0.74399999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>821</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1226</v>
-      </c>
-      <c r="C24">
-        <v>0.78900000000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>822</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1123</v>
-      </c>
-      <c r="C25">
-        <v>0.58399999999999996</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>824</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1176</v>
-      </c>
-      <c r="C26">
-        <v>0.68300000000000005</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>825</v>
-      </c>
-      <c r="B27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27">
-        <v>0.79300000000000004</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>827</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1224</v>
-      </c>
-      <c r="C28">
-        <v>0.90200000000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>830</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1220</v>
-      </c>
-      <c r="C29">
-        <v>0.34100000000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>831</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1184</v>
-      </c>
-      <c r="C30">
-        <v>0.56399999999999995</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>832</v>
+        <v>977</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>1154</v>
       </c>
       <c r="C31">
-        <v>0.91300000000000003</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.85099999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>833</v>
+        <v>844</v>
       </c>
       <c r="B32" t="s">
-        <v>1206</v>
+        <v>37</v>
       </c>
       <c r="C32">
-        <v>0.45200000000000001</v>
+        <v>0.84799999999999998</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>835</v>
+        <v>943</v>
       </c>
       <c r="B33" t="s">
-        <v>1243</v>
+        <v>39</v>
       </c>
       <c r="C33">
-        <v>0.82199999999999995</v>
+        <v>0.84699999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>836</v>
+        <v>790</v>
       </c>
       <c r="B34" t="s">
-        <v>1192</v>
+        <v>41</v>
       </c>
       <c r="C34">
-        <v>0.504</v>
+        <v>0.84599999999999997</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>837</v>
+        <v>853</v>
       </c>
       <c r="B35" t="s">
-        <v>1126</v>
+        <v>43</v>
       </c>
       <c r="C35">
-        <v>0.71899999999999997</v>
+        <v>0.84599999999999997</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>838</v>
+        <v>992</v>
       </c>
       <c r="B36" t="s">
-        <v>1253</v>
+        <v>44</v>
       </c>
       <c r="C36">
-        <v>0.71099999999999997</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>839</v>
+        <v>983</v>
       </c>
       <c r="B37" t="s">
-        <v>1231</v>
+        <v>1156</v>
       </c>
       <c r="C37">
-        <v>0.76300000000000001</v>
+        <v>0.83599999999999997</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>840</v>
+        <v>890</v>
       </c>
       <c r="B38" t="s">
-        <v>1225</v>
+        <v>46</v>
       </c>
       <c r="C38">
-        <v>0.81499999999999995</v>
+        <v>0.83099999999999996</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>841</v>
+        <v>791</v>
       </c>
       <c r="B39" t="s">
-        <v>1180</v>
+        <v>1166</v>
       </c>
       <c r="C39">
-        <v>0.63600000000000001</v>
+        <v>0.82699999999999996</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>844</v>
+        <v>835</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>1243</v>
       </c>
       <c r="C40">
-        <v>0.84799999999999998</v>
+        <v>0.82199999999999995</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>845</v>
+        <v>969</v>
       </c>
       <c r="B41" t="s">
-        <v>1050</v>
+        <v>48</v>
       </c>
       <c r="C41">
-        <v>0.873</v>
+        <v>0.82099999999999995</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>846</v>
+        <v>974</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C42">
-        <v>0.92</v>
+        <v>0.81599999999999995</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>847</v>
+        <v>813</v>
       </c>
       <c r="B43" t="s">
-        <v>1205</v>
+        <v>1121</v>
       </c>
       <c r="C43">
-        <v>0.46700000000000003</v>
+        <v>0.81499999999999995</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>1225</v>
       </c>
       <c r="C44">
-        <v>0.90100000000000002</v>
+        <v>0.81499999999999995</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>849</v>
+        <v>914</v>
       </c>
       <c r="B45" t="s">
-        <v>1241</v>
+        <v>1138</v>
       </c>
       <c r="C45">
-        <v>0.71699999999999997</v>
+        <v>0.81399999999999995</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>1392</v>
+        <v>924</v>
       </c>
       <c r="B46" t="s">
-        <v>1238</v>
+        <v>52</v>
       </c>
       <c r="C46">
-        <v>0.7</v>
+        <v>0.81399999999999995</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>851</v>
+        <v>926</v>
       </c>
       <c r="B47" t="s">
-        <v>1175</v>
+        <v>54</v>
       </c>
       <c r="C47">
-        <v>0.71699999999999997</v>
+        <v>0.81100000000000005</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>852</v>
+        <v>800</v>
       </c>
       <c r="B48" t="s">
-        <v>1128</v>
+        <v>1244</v>
       </c>
       <c r="C48">
-        <v>0.71099999999999997</v>
+        <v>0.80800000000000005</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>853</v>
+        <v>888</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C49">
-        <v>0.84599999999999997</v>
+        <v>0.80500000000000005</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>854</v>
+        <v>825</v>
       </c>
       <c r="B50" t="s">
-        <v>1177</v>
+        <v>58</v>
       </c>
       <c r="C50">
-        <v>0.68200000000000005</v>
+        <v>0.79300000000000004</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>856</v>
+        <v>931</v>
       </c>
       <c r="B51" t="s">
-        <v>1217</v>
+        <v>60</v>
       </c>
       <c r="C51">
-        <v>0.38100000000000001</v>
+        <v>0.79100000000000004</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>857</v>
+        <v>1026</v>
       </c>
       <c r="B52" t="s">
-        <v>24</v>
+        <v>1245</v>
       </c>
       <c r="C52">
-        <v>0.88500000000000001</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>858</v>
+        <v>821</v>
       </c>
       <c r="B53" t="s">
-        <v>1208</v>
+        <v>1226</v>
       </c>
       <c r="C53">
-        <v>0.435</v>
+        <v>0.78900000000000003</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>860</v>
+        <v>981</v>
       </c>
       <c r="B54" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C54">
-        <v>0.89200000000000002</v>
+        <v>0.78800000000000003</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>861</v>
+        <v>979</v>
       </c>
       <c r="B55" t="s">
-        <v>1127</v>
+        <v>64</v>
       </c>
       <c r="C55">
-        <v>0.72399999999999998</v>
+        <v>0.78600000000000003</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>865</v>
+        <v>927</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>1171</v>
       </c>
       <c r="C56">
-        <v>0.89300000000000002</v>
+        <v>0.78400000000000003</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>866</v>
+        <v>962</v>
       </c>
       <c r="B57" t="s">
-        <v>1178</v>
+        <v>1148</v>
       </c>
       <c r="C57">
-        <v>0.67400000000000004</v>
+        <v>0.78300000000000003</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>867</v>
+        <v>812</v>
       </c>
       <c r="B58" t="s">
-        <v>1049</v>
+        <v>66</v>
       </c>
       <c r="C58">
-        <v>0.875</v>
+        <v>0.78200000000000003</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>869</v>
+        <v>808</v>
       </c>
       <c r="B59" t="s">
-        <v>74</v>
+        <v>1227</v>
       </c>
       <c r="C59">
-        <v>0.745</v>
+        <v>0.77600000000000002</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>872</v>
+        <v>975</v>
       </c>
       <c r="B60" t="s">
-        <v>1183</v>
+        <v>1150</v>
       </c>
       <c r="C60">
-        <v>0.57299999999999995</v>
+        <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>875</v>
+        <v>1393</v>
       </c>
       <c r="B61" t="s">
-        <v>1207</v>
+        <v>1228</v>
       </c>
       <c r="C61">
-        <v>0.441</v>
+        <v>0.77400000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>876</v>
+        <v>948</v>
       </c>
       <c r="B62" t="s">
-        <v>1214</v>
+        <v>1142</v>
       </c>
       <c r="C62">
-        <v>0.39200000000000002</v>
+        <v>0.77300000000000002</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>879</v>
+        <v>944</v>
       </c>
       <c r="B63" t="s">
-        <v>35</v>
+        <v>1172</v>
       </c>
       <c r="C63">
-        <v>0.86</v>
+        <v>0.77100000000000002</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>881</v>
+        <v>980</v>
       </c>
       <c r="B64" t="s">
-        <v>1236</v>
+        <v>68</v>
       </c>
       <c r="C64">
-        <v>0.628</v>
+        <v>0.76900000000000002</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>883</v>
+        <v>1018</v>
       </c>
       <c r="B65" t="s">
-        <v>1212</v>
+        <v>1229</v>
       </c>
       <c r="C65">
-        <v>0.39600000000000002</v>
+        <v>0.76600000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>884</v>
+        <v>918</v>
       </c>
       <c r="B66" t="s">
-        <v>1249</v>
+        <v>1141</v>
       </c>
       <c r="C66">
-        <v>0.63800000000000001</v>
+        <v>0.76500000000000001</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>885</v>
+        <v>963</v>
       </c>
       <c r="B67" t="s">
-        <v>1129</v>
+        <v>1230</v>
       </c>
       <c r="C67">
-        <v>0.89100000000000001</v>
+        <v>0.76500000000000001</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>887</v>
+        <v>1030</v>
       </c>
       <c r="B68" t="s">
-        <v>1235</v>
+        <v>1246</v>
       </c>
       <c r="C68">
-        <v>0.61699999999999999</v>
+        <v>0.76400000000000001</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>888</v>
+        <v>839</v>
       </c>
       <c r="B69" t="s">
-        <v>56</v>
+        <v>1231</v>
       </c>
       <c r="C69">
-        <v>0.80500000000000005</v>
+        <v>0.76300000000000001</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>889</v>
+        <v>916</v>
       </c>
       <c r="B70" t="s">
-        <v>1233</v>
+        <v>70</v>
       </c>
       <c r="C70">
-        <v>0.47099999999999997</v>
+        <v>0.75700000000000001</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>890</v>
+        <v>947</v>
       </c>
       <c r="B71" t="s">
-        <v>46</v>
+        <v>1232</v>
       </c>
       <c r="C71">
-        <v>0.83099999999999996</v>
+        <v>0.75600000000000001</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>891</v>
+        <v>985</v>
       </c>
       <c r="B72" t="s">
-        <v>1131</v>
+        <v>1173</v>
       </c>
       <c r="C72">
-        <v>0.68400000000000005</v>
+        <v>0.75600000000000001</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>892</v>
+        <v>916</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="C73">
-        <v>0.91600000000000004</v>
+        <v>0.754</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>893</v>
+      <c r="A74" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B74" t="s">
-        <v>1134</v>
+        <v>1160</v>
       </c>
       <c r="C74">
-        <v>0.88800000000000001</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>895</v>
+        <v>795</v>
       </c>
       <c r="B75" t="s">
-        <v>1130</v>
+        <v>72</v>
       </c>
       <c r="C75">
-        <v>0.58599999999999997</v>
+        <v>0.749</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="B76" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C76">
-        <v>0.64200000000000002</v>
+        <v>0.749</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>898</v>
+        <v>869</v>
       </c>
       <c r="B77" t="s">
-        <v>1132</v>
+        <v>74</v>
       </c>
       <c r="C77">
-        <v>0.749</v>
+        <v>0.745</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>899</v>
+        <v>903</v>
       </c>
       <c r="B78" t="s">
-        <v>11</v>
+        <v>1136</v>
       </c>
       <c r="C78">
-        <v>0.90600000000000003</v>
+        <v>0.745</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>900</v>
+        <v>820</v>
       </c>
       <c r="B79" t="s">
-        <v>28</v>
+        <v>1247</v>
       </c>
       <c r="C79">
-        <v>0.88100000000000001</v>
+        <v>0.74399999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>902</v>
+        <v>934</v>
       </c>
       <c r="B80" t="s">
-        <v>1240</v>
+        <v>76</v>
       </c>
       <c r="C80">
-        <v>0.71499999999999997</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>903</v>
+        <v>1022</v>
       </c>
       <c r="B81" t="s">
-        <v>1136</v>
+        <v>78</v>
       </c>
       <c r="C81">
-        <v>0.745</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>904</v>
+        <v>964</v>
       </c>
       <c r="B82" t="s">
-        <v>1135</v>
+        <v>1248</v>
       </c>
       <c r="C82">
-        <v>0.89</v>
+        <v>0.73699999999999999</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>905</v>
+        <v>807</v>
       </c>
       <c r="B83" t="s">
-        <v>1188</v>
+        <v>79</v>
       </c>
       <c r="C83">
-        <v>0.53500000000000003</v>
+        <v>0.73499999999999999</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>906</v>
+        <v>806</v>
       </c>
       <c r="B84" t="s">
-        <v>1139</v>
+        <v>81</v>
       </c>
       <c r="C84">
-        <v>0.628</v>
+        <v>0.73399999999999999</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>907</v>
+        <v>796</v>
       </c>
       <c r="B85" t="s">
-        <v>1125</v>
+        <v>83</v>
       </c>
       <c r="C85">
-        <v>0.58399999999999996</v>
+        <v>0.72899999999999998</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>908</v>
+        <v>861</v>
       </c>
       <c r="B86" t="s">
-        <v>1137</v>
+        <v>1127</v>
       </c>
       <c r="C86">
-        <v>0.60699999999999998</v>
+        <v>0.72399999999999998</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>909</v>
+        <v>1009</v>
       </c>
       <c r="B87" t="s">
-        <v>1197</v>
+        <v>1163</v>
       </c>
       <c r="C87">
-        <v>0.48799999999999999</v>
+        <v>0.72199999999999998</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>912</v>
+        <v>1017</v>
       </c>
       <c r="B88" t="s">
-        <v>1159</v>
+        <v>85</v>
       </c>
       <c r="C88">
-        <v>0.89100000000000001</v>
+        <v>0.72199999999999998</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>914</v>
+        <v>1014</v>
       </c>
       <c r="B89" t="s">
-        <v>1138</v>
+        <v>1174</v>
       </c>
       <c r="C89">
-        <v>0.81399999999999995</v>
+        <v>0.72099999999999997</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>916</v>
+        <v>837</v>
       </c>
       <c r="B90" t="s">
-        <v>70</v>
+        <v>1126</v>
       </c>
       <c r="C90">
-        <v>0.754</v>
+        <v>0.71899999999999997</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>916</v>
+        <v>1001</v>
       </c>
       <c r="B91" t="s">
-        <v>70</v>
+        <v>1242</v>
       </c>
       <c r="C91">
-        <v>0.75700000000000001</v>
+        <v>0.71899999999999997</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>917</v>
+        <v>849</v>
       </c>
       <c r="B92" t="s">
-        <v>1140</v>
+        <v>1241</v>
       </c>
       <c r="C92">
-        <v>0.56899999999999995</v>
+        <v>0.71699999999999997</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>918</v>
+        <v>851</v>
       </c>
       <c r="B93" t="s">
-        <v>1141</v>
+        <v>1175</v>
       </c>
       <c r="C93">
-        <v>0.76500000000000001</v>
+        <v>0.71699999999999997</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>920</v>
+        <v>902</v>
       </c>
       <c r="B94" t="s">
-        <v>26</v>
+        <v>1240</v>
       </c>
       <c r="C94">
-        <v>0.88300000000000001</v>
+        <v>0.71499999999999997</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>922</v>
+        <v>993</v>
       </c>
       <c r="B95" t="s">
-        <v>1210</v>
+        <v>1239</v>
       </c>
       <c r="C95">
-        <v>0.41199999999999998</v>
+        <v>0.71399999999999997</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>923</v>
+        <v>838</v>
       </c>
       <c r="B96" t="s">
-        <v>1199</v>
+        <v>1253</v>
       </c>
       <c r="C96">
-        <v>0.48599999999999999</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.71099999999999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>924</v>
+        <v>852</v>
       </c>
       <c r="B97" t="s">
-        <v>52</v>
+        <v>1128</v>
       </c>
       <c r="C97">
-        <v>0.81399999999999995</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.71099999999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>925</v>
+        <v>1015</v>
       </c>
       <c r="B98" t="s">
-        <v>30</v>
+        <v>1164</v>
       </c>
       <c r="C98">
-        <v>0.875</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.70499999999999996</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>926</v>
+        <v>1392</v>
       </c>
       <c r="B99" t="s">
-        <v>54</v>
+        <v>1238</v>
       </c>
       <c r="C99">
-        <v>0.81100000000000005</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>927</v>
+        <v>997</v>
       </c>
       <c r="B100" t="s">
-        <v>1171</v>
+        <v>1252</v>
       </c>
       <c r="C100">
-        <v>0.78400000000000003</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+      <c r="D100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>928</v>
+        <v>937</v>
       </c>
       <c r="B101" t="s">
-        <v>1182</v>
+        <v>1145</v>
       </c>
       <c r="C101">
-        <v>0.61699999999999999</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.69799999999999995</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>930</v>
+        <v>945</v>
       </c>
       <c r="B102" t="s">
-        <v>87</v>
+        <v>1143</v>
       </c>
       <c r="C102">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.69799999999999995</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>931</v>
+        <v>1013</v>
       </c>
       <c r="B103" t="s">
-        <v>60</v>
+        <v>1165</v>
       </c>
       <c r="C103">
-        <v>0.79100000000000004</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.69799999999999995</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>932</v>
+        <v>1036</v>
       </c>
       <c r="B104" t="s">
-        <v>1194</v>
+        <v>1155</v>
       </c>
       <c r="C104">
-        <v>0.498</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.69399999999999995</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>934</v>
+        <v>969</v>
       </c>
       <c r="B105" t="s">
-        <v>76</v>
+        <v>1151</v>
       </c>
       <c r="C105">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>935</v>
+        <v>891</v>
       </c>
       <c r="B106" t="s">
-        <v>1211</v>
+        <v>1131</v>
       </c>
       <c r="C106">
-        <v>0.40699999999999997</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.68400000000000005</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>936</v>
+        <v>824</v>
       </c>
       <c r="B107" t="s">
-        <v>1146</v>
+        <v>1176</v>
       </c>
       <c r="C107">
-        <v>0.52400000000000002</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.68300000000000005</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>937</v>
+        <v>854</v>
       </c>
       <c r="B108" t="s">
-        <v>1145</v>
+        <v>1177</v>
       </c>
       <c r="C108">
-        <v>0.69799999999999995</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.68200000000000005</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>941</v>
+        <v>976</v>
       </c>
       <c r="B109" t="s">
-        <v>1198</v>
+        <v>1251</v>
       </c>
       <c r="C109">
-        <v>0.48699999999999999</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.67600000000000005</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>943</v>
+        <v>866</v>
       </c>
       <c r="B110" t="s">
-        <v>39</v>
+        <v>1178</v>
       </c>
       <c r="C110">
-        <v>0.84699999999999998</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>944</v>
+        <v>818</v>
       </c>
       <c r="B111" t="s">
-        <v>1172</v>
+        <v>1250</v>
       </c>
       <c r="C111">
-        <v>0.77100000000000002</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>945</v>
+        <v>1001</v>
       </c>
       <c r="B112" t="s">
-        <v>1143</v>
+        <v>1237</v>
       </c>
       <c r="C112">
-        <v>0.69799999999999995</v>
+        <v>0.66200000000000003</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>946</v>
+        <v>1027</v>
       </c>
       <c r="B113" t="s">
-        <v>1209</v>
+        <v>1167</v>
       </c>
       <c r="C113">
-        <v>0.41399999999999998</v>
+        <v>0.66100000000000003</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>947</v>
+        <v>930</v>
       </c>
       <c r="B114" t="s">
-        <v>1232</v>
+        <v>87</v>
       </c>
       <c r="C114">
-        <v>0.75600000000000001</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>948</v>
+        <v>967</v>
       </c>
       <c r="B115" t="s">
-        <v>1142</v>
+        <v>1153</v>
       </c>
       <c r="C115">
-        <v>0.77300000000000002</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>949</v>
+        <v>1003</v>
       </c>
       <c r="B116" t="s">
-        <v>1213</v>
+        <v>1161</v>
       </c>
       <c r="C116">
-        <v>0.39300000000000002</v>
+        <v>0.65800000000000003</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>950</v>
+        <v>1039</v>
       </c>
       <c r="B117" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C117">
-        <v>0.626</v>
+        <v>0.65800000000000003</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>952</v>
+        <v>897</v>
       </c>
       <c r="B118" t="s">
-        <v>1222</v>
+        <v>1133</v>
       </c>
       <c r="C118">
-        <v>0.33700000000000002</v>
+        <v>0.64200000000000002</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>954</v>
+        <v>884</v>
       </c>
       <c r="B119" t="s">
-        <v>1193</v>
+        <v>1249</v>
       </c>
       <c r="C119">
-        <v>0.504</v>
+        <v>0.63800000000000001</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>955</v>
+        <v>1033</v>
       </c>
       <c r="B120" t="s">
-        <v>1234</v>
+        <v>1169</v>
       </c>
       <c r="C120">
-        <v>0.61399999999999999</v>
+        <v>0.63800000000000001</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>956</v>
+        <v>841</v>
       </c>
       <c r="B121" t="s">
-        <v>2</v>
+        <v>1180</v>
       </c>
       <c r="C121">
-        <v>0.92100000000000004</v>
+        <v>0.63600000000000001</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>957</v>
+      <c r="A122" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B122" t="s">
-        <v>0</v>
+        <v>1144</v>
       </c>
       <c r="C122">
-        <v>0.95499999999999996</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>961</v>
+        <v>881</v>
       </c>
       <c r="B123" t="s">
-        <v>1147</v>
+        <v>1236</v>
       </c>
       <c r="C123">
-        <v>0.91</v>
+        <v>0.628</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>962</v>
+        <v>906</v>
       </c>
       <c r="B124" t="s">
-        <v>1148</v>
+        <v>1139</v>
       </c>
       <c r="C124">
-        <v>0.78300000000000003</v>
+        <v>0.628</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>963</v>
+        <v>950</v>
       </c>
       <c r="B125" t="s">
-        <v>1230</v>
+        <v>1181</v>
       </c>
       <c r="C125">
-        <v>0.76500000000000001</v>
+        <v>0.626</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>963</v>
+      <c r="A126" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B126" t="s">
-        <v>1152</v>
+        <v>723</v>
       </c>
       <c r="C126">
-        <v>0.49099999999999999</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>964</v>
+        <v>887</v>
       </c>
       <c r="B127" t="s">
-        <v>1248</v>
+        <v>1235</v>
       </c>
       <c r="C127">
-        <v>0.73699999999999999</v>
+        <v>0.61699999999999999</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>967</v>
+        <v>928</v>
       </c>
       <c r="B128" t="s">
-        <v>1153</v>
+        <v>1182</v>
       </c>
       <c r="C128">
-        <v>0.66</v>
+        <v>0.61699999999999999</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>968</v>
+        <v>1034</v>
       </c>
       <c r="B129" t="s">
-        <v>1149</v>
+        <v>1168</v>
       </c>
       <c r="C129">
-        <v>0.53700000000000003</v>
+        <v>0.61599999999999999</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>969</v>
+        <v>955</v>
       </c>
       <c r="B130" t="s">
-        <v>48</v>
+        <v>1234</v>
       </c>
       <c r="C130">
-        <v>0.82099999999999995</v>
+        <v>0.61399999999999999</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>969</v>
+        <v>908</v>
       </c>
       <c r="B131" t="s">
-        <v>1151</v>
+        <v>1137</v>
       </c>
       <c r="C131">
-        <v>0.68600000000000005</v>
+        <v>0.60699999999999998</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>974</v>
+        <v>1010</v>
       </c>
       <c r="B132" t="s">
-        <v>50</v>
+        <v>1162</v>
       </c>
       <c r="C132">
-        <v>0.81599999999999995</v>
+        <v>0.60699999999999998</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>975</v>
+        <v>895</v>
       </c>
       <c r="B133" t="s">
-        <v>1150</v>
+        <v>1130</v>
       </c>
       <c r="C133">
-        <v>0.77500000000000002</v>
+        <v>0.58599999999999997</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>976</v>
+        <v>822</v>
       </c>
       <c r="B134" t="s">
-        <v>1251</v>
+        <v>1123</v>
       </c>
       <c r="C134">
-        <v>0.67600000000000005</v>
+        <v>0.58399999999999996</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>977</v>
+        <v>907</v>
       </c>
       <c r="B135" t="s">
-        <v>1154</v>
+        <v>1125</v>
       </c>
       <c r="C135">
-        <v>0.85099999999999998</v>
+        <v>0.58399999999999996</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>979</v>
+        <v>872</v>
       </c>
       <c r="B136" t="s">
-        <v>64</v>
+        <v>1183</v>
       </c>
       <c r="C136">
-        <v>0.78600000000000003</v>
+        <v>0.57299999999999995</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>980</v>
+        <v>917</v>
       </c>
       <c r="B137" t="s">
-        <v>68</v>
+        <v>1140</v>
       </c>
       <c r="C137">
-        <v>0.76900000000000002</v>
+        <v>0.56899999999999995</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>981</v>
+        <v>831</v>
       </c>
       <c r="B138" t="s">
-        <v>62</v>
+        <v>1184</v>
       </c>
       <c r="C138">
-        <v>0.78800000000000003</v>
+        <v>0.56399999999999995</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>982</v>
+        <v>1040</v>
       </c>
       <c r="B139" t="s">
-        <v>1191</v>
+        <v>1185</v>
       </c>
       <c r="C139">
-        <v>0.50600000000000001</v>
+        <v>0.56100000000000005</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>983</v>
+        <v>809</v>
       </c>
       <c r="B140" t="s">
-        <v>1156</v>
+        <v>1122</v>
       </c>
       <c r="C140">
-        <v>0.83599999999999997</v>
+        <v>0.55800000000000005</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>985</v>
+        <v>999</v>
       </c>
       <c r="B141" t="s">
-        <v>1173</v>
+        <v>1186</v>
       </c>
       <c r="C141">
-        <v>0.75600000000000001</v>
+        <v>0.55800000000000005</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
-        <v>986</v>
+      <c r="A142" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B142" t="s">
-        <v>1203</v>
+        <v>1187</v>
       </c>
       <c r="C142">
-        <v>0.47299999999999998</v>
+        <v>0.55600000000000005</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>987</v>
+      <c r="A143" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B143" t="s">
-        <v>8</v>
+        <v>1042</v>
       </c>
       <c r="C143">
-        <v>0.91600000000000004</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>988</v>
+        <v>968</v>
       </c>
       <c r="B144" t="s">
-        <v>1157</v>
+        <v>1149</v>
       </c>
       <c r="C144">
-        <v>0.90100000000000002</v>
+        <v>0.53700000000000003</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>990</v>
+        <v>905</v>
       </c>
       <c r="B145" t="s">
-        <v>23</v>
+        <v>1188</v>
       </c>
       <c r="C145">
-        <v>0.89200000000000002</v>
+        <v>0.53500000000000003</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>992</v>
+        <v>1004</v>
       </c>
       <c r="B146" t="s">
-        <v>44</v>
+        <v>1189</v>
       </c>
       <c r="C146">
-        <v>0.84</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>993</v>
+        <v>798</v>
       </c>
       <c r="B147" t="s">
-        <v>1218</v>
+        <v>1190</v>
       </c>
       <c r="C147">
-        <v>0.374</v>
+        <v>0.52600000000000002</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>993</v>
+        <v>936</v>
       </c>
       <c r="B148" t="s">
-        <v>1239</v>
+        <v>1146</v>
       </c>
       <c r="C148">
-        <v>0.71399999999999997</v>
+        <v>0.52400000000000002</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>995</v>
+        <v>982</v>
       </c>
       <c r="B149" t="s">
-        <v>1200</v>
+        <v>1191</v>
       </c>
       <c r="C149">
-        <v>0.48499999999999999</v>
+        <v>0.50600000000000001</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>997</v>
+        <v>836</v>
       </c>
       <c r="B150" t="s">
-        <v>1252</v>
+        <v>1192</v>
       </c>
       <c r="C150">
-        <v>0.7</v>
+        <v>0.504</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>999</v>
+        <v>954</v>
       </c>
       <c r="B151" t="s">
-        <v>1186</v>
+        <v>1193</v>
       </c>
       <c r="C151">
-        <v>0.55800000000000005</v>
+        <v>0.504</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>1001</v>
+        <v>1037</v>
       </c>
       <c r="B152" t="s">
-        <v>1237</v>
+        <v>1170</v>
       </c>
       <c r="C152">
-        <v>0.66200000000000003</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>1001</v>
+        <v>932</v>
       </c>
       <c r="B153" t="s">
-        <v>1242</v>
+        <v>1194</v>
       </c>
       <c r="C153">
-        <v>0.71899999999999997</v>
+        <v>0.498</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>1003</v>
+        <v>1041</v>
       </c>
       <c r="B154" t="s">
-        <v>1161</v>
+        <v>1195</v>
       </c>
       <c r="C154">
-        <v>0.65800000000000003</v>
+        <v>0.49199999999999999</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>1004</v>
+        <v>963</v>
       </c>
       <c r="B155" t="s">
-        <v>1189</v>
+        <v>1152</v>
       </c>
       <c r="C155">
-        <v>0.53</v>
+        <v>0.49099999999999999</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
-        <v>1006</v>
+      <c r="A156" t="e">
+        <v>#N/A</v>
       </c>
       <c r="B156" t="s">
-        <v>1219</v>
+        <v>1158</v>
       </c>
       <c r="C156">
-        <v>0.372</v>
+        <v>0.49099999999999999</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>1008</v>
+        <v>909</v>
       </c>
       <c r="B157" t="s">
-        <v>1204</v>
+        <v>1197</v>
       </c>
       <c r="C157">
-        <v>0.47299999999999998</v>
+        <v>0.48799999999999999</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>1009</v>
+        <v>1021</v>
       </c>
       <c r="B158" t="s">
-        <v>1163</v>
+        <v>1196</v>
       </c>
       <c r="C158">
-        <v>0.72199999999999998</v>
+        <v>0.48799999999999999</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>1010</v>
+        <v>941</v>
       </c>
       <c r="B159" t="s">
-        <v>1162</v>
+        <v>1198</v>
       </c>
       <c r="C159">
-        <v>0.60699999999999998</v>
+        <v>0.48699999999999999</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>1013</v>
+        <v>923</v>
       </c>
       <c r="B160" t="s">
-        <v>1165</v>
+        <v>1199</v>
       </c>
       <c r="C160">
-        <v>0.69799999999999995</v>
+        <v>0.48599999999999999</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>1014</v>
+        <v>995</v>
       </c>
       <c r="B161" t="s">
-        <v>1174</v>
+        <v>1200</v>
       </c>
       <c r="C161">
-        <v>0.72099999999999997</v>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>1015</v>
+        <v>1023</v>
       </c>
       <c r="B162" t="s">
-        <v>1164</v>
+        <v>1201</v>
       </c>
       <c r="C162">
-        <v>0.70499999999999996</v>
+        <v>0.48399999999999999</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>1017</v>
+        <v>815</v>
       </c>
       <c r="B163" t="s">
-        <v>85</v>
+        <v>1202</v>
       </c>
       <c r="C163">
-        <v>0.72199999999999998</v>
+        <v>0.47599999999999998</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>1018</v>
+        <v>986</v>
       </c>
       <c r="B164" t="s">
-        <v>1229</v>
+        <v>1203</v>
       </c>
       <c r="C164">
-        <v>0.76600000000000001</v>
+        <v>0.47299999999999998</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>1021</v>
+        <v>1008</v>
       </c>
       <c r="B165" t="s">
-        <v>1196</v>
+        <v>1204</v>
       </c>
       <c r="C165">
-        <v>0.48799999999999999</v>
+        <v>0.47299999999999998</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>1022</v>
+        <v>889</v>
       </c>
       <c r="B166" t="s">
-        <v>78</v>
+        <v>1233</v>
       </c>
       <c r="C166">
-        <v>0.74</v>
+        <v>0.47099999999999997</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>1023</v>
+        <v>792</v>
       </c>
       <c r="B167" t="s">
-        <v>1201</v>
+        <v>1119</v>
       </c>
       <c r="C167">
-        <v>0.48399999999999999</v>
+        <v>0.46800000000000003</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>1025</v>
+        <v>847</v>
       </c>
       <c r="B168" t="s">
-        <v>1223</v>
+        <v>1205</v>
       </c>
       <c r="C168">
-        <v>0.91400000000000003</v>
+        <v>0.46700000000000003</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>1026</v>
+        <v>833</v>
       </c>
       <c r="B169" t="s">
-        <v>1245</v>
+        <v>1206</v>
       </c>
       <c r="C169">
-        <v>0.79</v>
+        <v>0.45200000000000001</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>1027</v>
+        <v>875</v>
       </c>
       <c r="B170" t="s">
-        <v>1167</v>
+        <v>1207</v>
       </c>
       <c r="C170">
-        <v>0.66100000000000003</v>
+        <v>0.441</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>1030</v>
+        <v>858</v>
       </c>
       <c r="B171" t="s">
-        <v>1246</v>
+        <v>1208</v>
       </c>
       <c r="C171">
-        <v>0.76400000000000001</v>
+        <v>0.435</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>1033</v>
+        <v>946</v>
       </c>
       <c r="B172" t="s">
-        <v>1169</v>
+        <v>1209</v>
       </c>
       <c r="C172">
-        <v>0.63800000000000001</v>
+        <v>0.41399999999999998</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>1034</v>
+        <v>922</v>
       </c>
       <c r="B173" t="s">
-        <v>1168</v>
+        <v>1210</v>
       </c>
       <c r="C173">
-        <v>0.61599999999999999</v>
+        <v>0.41199999999999998</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>1036</v>
+        <v>935</v>
       </c>
       <c r="B174" t="s">
-        <v>1155</v>
+        <v>1211</v>
       </c>
       <c r="C174">
-        <v>0.69399999999999995</v>
+        <v>0.40699999999999997</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>1037</v>
+        <v>883</v>
       </c>
       <c r="B175" t="s">
-        <v>1170</v>
+        <v>1212</v>
       </c>
       <c r="C175">
-        <v>0.5</v>
+        <v>0.39600000000000002</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>1039</v>
+        <v>949</v>
       </c>
       <c r="B176" t="s">
-        <v>1179</v>
+        <v>1213</v>
       </c>
       <c r="C176">
-        <v>0.65800000000000003</v>
+        <v>0.39300000000000002</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>1040</v>
+        <v>876</v>
       </c>
       <c r="B177" t="s">
-        <v>1185</v>
+        <v>1214</v>
       </c>
       <c r="C177">
-        <v>0.56100000000000005</v>
+        <v>0.39200000000000002</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>1041</v>
+        <v>814</v>
       </c>
       <c r="B178" t="s">
-        <v>1195</v>
+        <v>1215</v>
       </c>
       <c r="C178">
-        <v>0.49199999999999999</v>
+        <v>0.38900000000000001</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179" t="e">
-        <v>#N/A</v>
+      <c r="A179" t="s">
+        <v>811</v>
       </c>
       <c r="B179" t="s">
-        <v>1144</v>
+        <v>1216</v>
       </c>
       <c r="C179">
-        <v>0.63</v>
+        <v>0.38800000000000001</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A180" t="e">
-        <v>#N/A</v>
+      <c r="A180" t="s">
+        <v>856</v>
       </c>
       <c r="B180" t="s">
-        <v>1042</v>
+        <v>1217</v>
       </c>
       <c r="C180">
-        <v>0.54</v>
+        <v>0.38100000000000001</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A181" t="e">
-        <v>#N/A</v>
+      <c r="A181" t="s">
+        <v>993</v>
       </c>
       <c r="B181" t="s">
-        <v>1158</v>
+        <v>1218</v>
       </c>
       <c r="C181">
-        <v>0.49099999999999999</v>
+        <v>0.374</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A182" t="e">
-        <v>#N/A</v>
+      <c r="A182" t="s">
+        <v>1006</v>
       </c>
       <c r="B182" t="s">
-        <v>1160</v>
+        <v>1219</v>
       </c>
       <c r="C182">
-        <v>0.75</v>
+        <v>0.372</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A183" t="e">
-        <v>#N/A</v>
+      <c r="A183" t="s">
+        <v>830</v>
       </c>
       <c r="B183" t="s">
-        <v>723</v>
+        <v>1220</v>
       </c>
       <c r="C183">
-        <v>0.62</v>
+        <v>0.34100000000000003</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
@@ -50949,24 +50961,27 @@
         <v>#N/A</v>
       </c>
       <c r="B184" t="s">
-        <v>1187</v>
+        <v>1221</v>
       </c>
       <c r="C184">
-        <v>0.55600000000000005</v>
+        <v>0.33800000000000002</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A185" t="e">
-        <v>#N/A</v>
+      <c r="A185" t="s">
+        <v>952</v>
       </c>
       <c r="B185" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="C185">
-        <v>0.33800000000000002</v>
+        <v>0.33700000000000002</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:C185">
+    <sortCondition descending="1" ref="C1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>